<commit_message>
agregando DER y MODELO MVC
</commit_message>
<xml_diff>
--- a/wireframes/descripcion-modelos.xlsx
+++ b/wireframes/descripcion-modelos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DER" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="73">
   <si>
     <t>id_usuario</t>
   </si>
@@ -98,9 +98,6 @@
   </si>
   <si>
     <t>AMIGO</t>
-  </si>
-  <si>
-    <t>id_jugador</t>
   </si>
   <si>
     <t>alias</t>
@@ -176,6 +173,93 @@
   <si>
     <t>finalizado_exito</t>
   </si>
+  <si>
+    <t>USUARIO</t>
+  </si>
+  <si>
+    <t>INDEX.php</t>
+  </si>
+  <si>
+    <t>SESSION.CONTROLLER</t>
+  </si>
+  <si>
+    <t>USUARIO.MODEL</t>
+  </si>
+  <si>
+    <t>IniciarSession()</t>
+  </si>
+  <si>
+    <t>PARTIDA.CONTROLLER</t>
+  </si>
+  <si>
+    <t>PARTIDA.MODEL</t>
+  </si>
+  <si>
+    <t>nuevaPartida()</t>
+  </si>
+  <si>
+    <t>retomarPartida()</t>
+  </si>
+  <si>
+    <t>abandonarPartida()</t>
+  </si>
+  <si>
+    <t>listarPartidas()</t>
+  </si>
+  <si>
+    <t>agregarMovimiento()</t>
+  </si>
+  <si>
+    <t>controlarMovimiento()</t>
+  </si>
+  <si>
+    <t>VIEWS</t>
+  </si>
+  <si>
+    <t>listadoPartidasView</t>
+  </si>
+  <si>
+    <t>jugarPartidaView</t>
+  </si>
+  <si>
+    <t>configurarPartidaView</t>
+  </si>
+  <si>
+    <t>verPartidaIniciada</t>
+  </si>
+  <si>
+    <t>listadoPartidas: (array)</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int </t>
+  </si>
+  <si>
+    <t>contraseña</t>
+  </si>
+  <si>
+    <t>int : FK</t>
+  </si>
+  <si>
+    <t>blob</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>json</t>
+  </si>
+  <si>
+    <t>estado_inicial</t>
+  </si>
 </sst>
 </file>
 
@@ -198,7 +282,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -220,12 +304,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -294,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -302,22 +380,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -330,6 +392,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -338,6 +403,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -350,6 +418,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -654,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,36 +770,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="D1" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="10"/>
-      <c r="H1" s="10" t="s">
+      <c r="B1" s="15"/>
+      <c r="D1" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="15"/>
+      <c r="H1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="L1" s="10" t="s">
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="L1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="V1" s="20" t="s">
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="V1" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="20"/>
-      <c r="X1" s="20"/>
-      <c r="Y1" s="20"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -725,16 +809,16 @@
         <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>14</v>
@@ -746,19 +830,19 @@
         <v>1</v>
       </c>
       <c r="N2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="P2" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>2</v>
+        <v>72</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>2</v>
@@ -787,7 +871,7 @@
         <v>23185125</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" s="1"/>
       <c r="H3" s="1">
@@ -806,13 +890,13 @@
         <v>1</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q3" s="6">
         <v>44000</v>
@@ -847,7 +931,7 @@
         <v>54866263</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" s="1"/>
       <c r="H4" s="1">
@@ -862,13 +946,13 @@
         <v>2</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q4" s="6">
         <v>43997</v>
@@ -877,7 +961,7 @@
         <v>7</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T4" s="5">
         <v>1</v>
@@ -903,7 +987,7 @@
         <v>22477522</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" s="1"/>
       <c r="H5" s="1"/>
@@ -916,13 +1000,13 @@
         <v>3</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q5" s="6">
         <v>43993</v>
@@ -931,7 +1015,7 @@
         <v>7</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="T5" s="5">
         <v>2</v>
@@ -1048,10 +1132,10 @@
       <c r="Y12" s="4"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="13"/>
+      <c r="B13" s="7"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="H13" s="11" t="s">
@@ -1070,219 +1154,185 @@
       <c r="R13" s="11"/>
       <c r="S13" s="11"/>
       <c r="T13" s="11"/>
-      <c r="V13" s="14" t="s">
+      <c r="V13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="W13" s="15"/>
-      <c r="X13" s="15"/>
-      <c r="Y13" s="16"/>
+      <c r="W13" s="9"/>
+      <c r="X13" s="9"/>
+      <c r="Y13" s="10"/>
     </row>
     <row r="14" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="20"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="H14" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="18"/>
+      <c r="J14" s="19"/>
+      <c r="L14" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
+      <c r="V14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="W14" s="9"/>
+      <c r="X14" s="9"/>
+      <c r="Y14" s="10"/>
+    </row>
+    <row r="15" spans="1:26" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="20"/>
+      <c r="B15" s="20"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="H15" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" s="13"/>
+      <c r="J15" s="14"/>
+      <c r="L15" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+      <c r="V15" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="W15" s="9"/>
+      <c r="X15" s="9"/>
+      <c r="Y15" s="10"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16" s="20"/>
+      <c r="B16" s="20"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="14"/>
+      <c r="L16" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="9"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="H14" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="I14" s="22"/>
-      <c r="J14" s="23"/>
-      <c r="L14" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="13"/>
-      <c r="R14" s="13"/>
-      <c r="S14" s="13"/>
-      <c r="T14" s="13"/>
-      <c r="V14" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="W14" s="15"/>
-      <c r="X14" s="15"/>
-      <c r="Y14" s="16"/>
-    </row>
-    <row r="15" spans="1:26" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="H15" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="I15" s="18"/>
-      <c r="J15" s="19"/>
-      <c r="L15" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="13"/>
-      <c r="R15" s="13"/>
-      <c r="S15" s="13"/>
-      <c r="T15" s="13"/>
-      <c r="V15" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="W15" s="15"/>
-      <c r="X15" s="15"/>
-      <c r="Y15" s="16"/>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="19"/>
-      <c r="L16" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
-      <c r="P16" s="13"/>
-      <c r="Q16" s="13"/>
-      <c r="R16" s="13"/>
-      <c r="S16" s="13"/>
-      <c r="T16" s="13"/>
-      <c r="V16" s="14"/>
-      <c r="W16" s="15"/>
-      <c r="X16" s="15"/>
-      <c r="Y16" s="16"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
+      <c r="V16" s="8"/>
+      <c r="W16" s="9"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="10"/>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="19"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="13"/>
-      <c r="Q17" s="13"/>
-      <c r="R17" s="13"/>
-      <c r="S17" s="13"/>
-      <c r="T17" s="13"/>
-      <c r="V17" s="14"/>
-      <c r="W17" s="15"/>
-      <c r="X17" s="15"/>
-      <c r="Y17" s="16"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="20"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="14"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+      <c r="V17" s="8"/>
+      <c r="W17" s="9"/>
+      <c r="X17" s="9"/>
+      <c r="Y17" s="10"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="19"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="13"/>
-      <c r="R18" s="13"/>
-      <c r="S18" s="13"/>
-      <c r="T18" s="13"/>
-      <c r="V18" s="14"/>
-      <c r="W18" s="15"/>
-      <c r="X18" s="15"/>
-      <c r="Y18" s="16"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="20"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="14"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
+      <c r="V18" s="8"/>
+      <c r="W18" s="9"/>
+      <c r="X18" s="9"/>
+      <c r="Y18" s="10"/>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="19"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="13"/>
-      <c r="Q19" s="13"/>
-      <c r="R19" s="13"/>
-      <c r="S19" s="13"/>
-      <c r="T19" s="13"/>
-      <c r="V19" s="14"/>
-      <c r="W19" s="15"/>
-      <c r="X19" s="15"/>
-      <c r="Y19" s="16"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="20"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="14"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="V19" s="8"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="9"/>
+      <c r="Y19" s="10"/>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="19"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="13"/>
-      <c r="R20" s="13"/>
-      <c r="S20" s="13"/>
-      <c r="T20" s="13"/>
-      <c r="V20" s="14"/>
-      <c r="W20" s="15"/>
-      <c r="X20" s="15"/>
-      <c r="Y20" s="16"/>
+      <c r="A20" s="20"/>
+      <c r="B20" s="20"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="14"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
+      <c r="V20" s="8"/>
+      <c r="W20" s="9"/>
+      <c r="X20" s="9"/>
+      <c r="Y20" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="L16:T16"/>
-    <mergeCell ref="L17:T17"/>
-    <mergeCell ref="V20:Y20"/>
-    <mergeCell ref="L13:T13"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="L1:T1"/>
-    <mergeCell ref="V13:Y13"/>
-    <mergeCell ref="V14:Y14"/>
-    <mergeCell ref="V15:Y15"/>
-    <mergeCell ref="V16:Y16"/>
-    <mergeCell ref="V17:Y17"/>
-    <mergeCell ref="V18:Y18"/>
-    <mergeCell ref="V19:Y19"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="L18:T18"/>
-    <mergeCell ref="L19:T19"/>
-    <mergeCell ref="L20:T20"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="L14:T14"/>
-    <mergeCell ref="L15:T15"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A20:B20"/>
@@ -1294,6 +1344,40 @@
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="D19:E19"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="L18:T18"/>
+    <mergeCell ref="L19:T19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="L14:T14"/>
+    <mergeCell ref="L15:T15"/>
+    <mergeCell ref="L1:T1"/>
+    <mergeCell ref="V13:Y13"/>
+    <mergeCell ref="V14:Y14"/>
+    <mergeCell ref="V15:Y15"/>
+    <mergeCell ref="V16:Y16"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="L16:T16"/>
+    <mergeCell ref="L17:T17"/>
+    <mergeCell ref="V20:Y20"/>
+    <mergeCell ref="L13:T13"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="V17:Y17"/>
+    <mergeCell ref="V18:Y18"/>
+    <mergeCell ref="V19:Y19"/>
+    <mergeCell ref="L20:T20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1302,28 +1386,91 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:E5"/>
+  <dimension ref="B3:N9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3:N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" t="s">
-        <v>28</v>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="H4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L8" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L9" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1333,12 +1480,236 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="D1" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="16"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="15"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="25"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="15"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="26"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>